<commit_message>
Complete - Post Walkthrough
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17033\Documents\Data Analytics 14\Projects\lookups-da14-jmo703\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A28D2C-441A-4582-B84D-675A7E407B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888C9A16-DC57-4519-9327-951FFFFA76F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -808,7 +830,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -821,6 +843,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1861,16 +1886,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>655320</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>37147</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>159067</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1638300</xdr:colOff>
-      <xdr:row>87</xdr:row>
-      <xdr:rowOff>63817</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>2857</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2197,8 +2222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="F107" sqref="F107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2280,12 +2305,12 @@
         <v>-15396420.870000005</v>
       </c>
       <c r="E2" s="5">
-        <f>D2/B2</f>
+        <f>IFERROR((D2/B2),"0.00"%)</f>
         <v>-4.3170750765267295E-2</v>
       </c>
       <c r="F2">
-        <f>IFERROR(RANK(E2,$E$2:$E$52), "Not Found")</f>
-        <v>35</v>
+        <f>IFERROR(RANK(E2,$E$2:$E$52,1), "Not Found")</f>
+        <v>14</v>
       </c>
       <c r="G2">
         <v>382685200</v>
@@ -2297,13 +2322,13 @@
         <f>(H2-G2)</f>
         <v>-36344389.180000007</v>
       </c>
-      <c r="J2" s="5">
-        <f>(I2/G2)</f>
+      <c r="J2" s="10">
+        <f>IFERROR((I2/G2),"0.00%")</f>
         <v>-9.4972027086493035E-2</v>
       </c>
       <c r="K2">
-        <f>IFERROR(RANK(J2,$J$2:$J$52), "Not Found")</f>
-        <v>39</v>
+        <f>IFERROR(RANK(J2,$J$2:$J$52,1), "Not Found")</f>
+        <v>10</v>
       </c>
       <c r="L2">
         <v>376548600</v>
@@ -2315,13 +2340,13 @@
         <f>(M2-L2)</f>
         <v>-21269107.770000994</v>
       </c>
-      <c r="O2" s="5">
-        <f>IFERROR(N2/L2, "Not Found")</f>
+      <c r="O2" s="10">
+        <f>IFERROR(N2/L2, "0.00%")</f>
         <v>-5.6484362894991494E-2</v>
       </c>
       <c r="P2">
-        <f>IFERROR(RANK(O2,$O$2:$O$52),"Not Found")</f>
-        <v>35</v>
+        <f>IFERROR(RANK(O2,$O$2:$O$52,1),"Not Found")</f>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -2339,12 +2364,12 @@
         <v>-7585.4099999999744</v>
       </c>
       <c r="E3" s="5">
-        <f t="shared" ref="E3:E10" si="1">D3/B3</f>
+        <f t="shared" ref="E3:E52" si="1">IFERROR((D3/B3),"0.00"%)</f>
         <v>-2.3069981751824741E-2</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F52" si="2">IFERROR(RANK(E3,$E$2:$E$52), "Not Found")</f>
-        <v>27</v>
+        <f t="shared" ref="F3:F52" si="2">IFERROR(RANK(E3,$E$2:$E$52,1), "Not Found")</f>
+        <v>22</v>
       </c>
       <c r="G3">
         <v>334800</v>
@@ -2356,13 +2381,13 @@
         <f t="shared" ref="I3:I52" si="3">(H3-G3)</f>
         <v>-22366.290000001027</v>
       </c>
-      <c r="J3" s="5">
-        <f t="shared" ref="J3:J10" si="4">(I3/G3)</f>
+      <c r="J3" s="10">
+        <f t="shared" ref="J3:J52" si="4">IFERROR((I3/G3),"0.00%")</f>
         <v>-6.6804928315415249E-2</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K52" si="5">IFERROR(RANK(J3,$J$2:$J$52), "Not Found")</f>
-        <v>35</v>
+        <f t="shared" ref="K3:K52" si="5">IFERROR(RANK(J3,$J$2:$J$52,1), "Not Found")</f>
+        <v>14</v>
       </c>
       <c r="L3">
         <v>322700</v>
@@ -2374,13 +2399,13 @@
         <f t="shared" ref="N3:N52" si="6">(M3-L3)</f>
         <v>-436.96000000002095</v>
       </c>
-      <c r="O3" s="5">
-        <f t="shared" ref="O3:O52" si="7">IFERROR(N3/L3, "Not Found")</f>
+      <c r="O3" s="10">
+        <f t="shared" ref="O3:O52" si="7">IFERROR(N3/L3, "0.00%")</f>
         <v>-1.3540749922529313E-3</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P52" si="8">IFERROR(RANK(O3,$O$2:$O$52),"Not Found")</f>
-        <v>12</v>
+        <f t="shared" ref="P3:P52" si="8">IFERROR(RANK(O3,$O$2:$O$52,1),"Not Found")</f>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -2403,7 +2428,7 @@
       </c>
       <c r="F4">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="G4">
         <v>3652300</v>
@@ -2415,13 +2440,13 @@
         <f t="shared" si="3"/>
         <v>-62606.790000009816</v>
       </c>
-      <c r="J4" s="5">
-        <f>(I4/G4)</f>
+      <c r="J4" s="10">
+        <f t="shared" si="4"/>
         <v>-1.7141743558856015E-2</v>
       </c>
       <c r="K4">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="L4">
         <v>3662400</v>
@@ -2433,13 +2458,13 @@
         <f t="shared" si="6"/>
         <v>-97416.950000009965</v>
       </c>
-      <c r="O4" s="5">
+      <c r="O4" s="10">
         <f t="shared" si="7"/>
         <v>-2.6599210899959033E-2</v>
       </c>
       <c r="P4">
         <f t="shared" si="8"/>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -2462,7 +2487,7 @@
       </c>
       <c r="F5">
         <f t="shared" si="2"/>
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="G5">
         <v>7968300</v>
@@ -2474,13 +2499,13 @@
         <f t="shared" si="3"/>
         <v>-947690.6799999997</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="10">
         <f t="shared" si="4"/>
         <v>-0.118932605449092</v>
       </c>
       <c r="K5">
         <f t="shared" si="5"/>
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="L5">
         <v>7759600</v>
@@ -2492,13 +2517,13 @@
         <f t="shared" si="6"/>
         <v>-262277.08999999985</v>
       </c>
-      <c r="O5" s="5">
+      <c r="O5" s="10">
         <f t="shared" si="7"/>
         <v>-3.3800336357544182E-2</v>
       </c>
       <c r="P5">
         <f t="shared" si="8"/>
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
@@ -2521,7 +2546,7 @@
       </c>
       <c r="F6">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="G6">
         <v>428500</v>
@@ -2533,13 +2558,13 @@
         <f t="shared" si="3"/>
         <v>-741.35999999998603</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="10">
         <f t="shared" si="4"/>
         <v>-1.7301283547257551E-3</v>
       </c>
       <c r="K6">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="L6">
         <v>445200</v>
@@ -2551,13 +2576,13 @@
         <f t="shared" si="6"/>
         <v>-85.710000001010485</v>
       </c>
-      <c r="O6" s="5">
+      <c r="O6" s="10">
         <f t="shared" si="7"/>
         <v>-1.925202156356929E-4</v>
       </c>
       <c r="P6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -2580,7 +2605,7 @@
       </c>
       <c r="F7">
         <f t="shared" si="2"/>
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="G7">
         <v>3390900</v>
@@ -2592,13 +2617,13 @@
         <f t="shared" si="3"/>
         <v>-339416.58999999985</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="10">
         <f t="shared" si="4"/>
         <v>-0.10009631366303927</v>
       </c>
       <c r="K7">
         <f t="shared" si="5"/>
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="L7">
         <v>3345200</v>
@@ -2610,13 +2635,13 @@
         <f t="shared" si="6"/>
         <v>-398759.91999999993</v>
       </c>
-      <c r="O7" s="5">
+      <c r="O7" s="10">
         <f t="shared" si="7"/>
         <v>-0.11920361114432618</v>
       </c>
       <c r="P7">
         <f t="shared" si="8"/>
-        <v>45</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
@@ -2639,7 +2664,7 @@
       </c>
       <c r="F8">
         <f t="shared" si="2"/>
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <v>1590700</v>
@@ -2651,13 +2676,13 @@
         <f t="shared" si="3"/>
         <v>-206794.01000001002</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="10">
         <f t="shared" si="4"/>
         <v>-0.13000189224870184</v>
       </c>
       <c r="K8">
         <f t="shared" si="5"/>
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="L8">
         <v>1579300</v>
@@ -2669,13 +2694,13 @@
         <f t="shared" si="6"/>
         <v>-241564.68000000995</v>
       </c>
-      <c r="O8" s="5">
+      <c r="O8" s="10">
         <f t="shared" si="7"/>
         <v>-0.15295680364719175</v>
       </c>
       <c r="P8">
         <f t="shared" si="8"/>
-        <v>47</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
@@ -2698,7 +2723,7 @@
       </c>
       <c r="F9">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="G9">
         <v>11073700</v>
@@ -2710,13 +2735,13 @@
         <f t="shared" si="3"/>
         <v>-1144640.4800000004</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="10">
         <f t="shared" si="4"/>
         <v>-0.10336567542917005</v>
       </c>
       <c r="K9">
         <f t="shared" si="5"/>
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="L9">
         <v>10790500</v>
@@ -2728,13 +2753,13 @@
         <f t="shared" si="6"/>
         <v>-796900.47000000998</v>
       </c>
-      <c r="O9" s="5">
+      <c r="O9" s="10">
         <f t="shared" si="7"/>
         <v>-7.3852043000788653E-2</v>
       </c>
       <c r="P9">
         <f t="shared" si="8"/>
-        <v>40</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
@@ -2757,7 +2782,7 @@
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="G10">
         <v>495200</v>
@@ -2769,13 +2794,13 @@
         <f t="shared" si="3"/>
         <v>-27292.159999999974</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="10">
         <f t="shared" si="4"/>
         <v>-5.5113408723747932E-2</v>
       </c>
       <c r="K10">
         <f t="shared" si="5"/>
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="L10">
         <v>487500</v>
@@ -2787,13 +2812,13 @@
         <f t="shared" si="6"/>
         <v>-9181.0800000000163</v>
       </c>
-      <c r="O10" s="5">
+      <c r="O10" s="10">
         <f t="shared" si="7"/>
         <v>-1.883298461538465E-2</v>
       </c>
       <c r="P10">
         <f t="shared" si="8"/>
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -2810,13 +2835,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E11" s="5" t="str">
-        <f>IFERROR(D11/B11,"Not Found")</f>
-        <v>Not Found</v>
-      </c>
-      <c r="F11" t="str">
+      <c r="E11" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F11">
         <f t="shared" si="2"/>
-        <v>Not Found</v>
+        <v>47</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -2828,13 +2853,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J11" s="5" t="str">
-        <f>IFERROR(I11/G11, "Not Found")</f>
-        <v>Not Found</v>
-      </c>
-      <c r="K11" t="str">
+      <c r="J11" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>0.00%</v>
+      </c>
+      <c r="K11">
         <f t="shared" si="5"/>
-        <v>Not Found</v>
+        <v>48</v>
       </c>
       <c r="L11">
         <v>375000</v>
@@ -2846,13 +2871,13 @@
         <f t="shared" si="6"/>
         <v>-311228.08999999997</v>
       </c>
-      <c r="O11" s="5">
+      <c r="O11" s="10">
         <f t="shared" si="7"/>
         <v>-0.82994157333333329</v>
       </c>
       <c r="P11">
         <f t="shared" si="8"/>
-        <v>48</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
@@ -2870,12 +2895,12 @@
         <v>-214304.66999999993</v>
       </c>
       <c r="E12" s="5">
-        <f t="shared" ref="E12:E52" si="9">IFERROR(D12/B12,"Not Found")</f>
+        <f t="shared" si="1"/>
         <v>-5.0060657805601608E-2</v>
       </c>
       <c r="F12">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="G12">
         <v>4700400</v>
@@ -2887,13 +2912,13 @@
         <f t="shared" si="3"/>
         <v>-494844.40000000037</v>
       </c>
-      <c r="J12" s="5">
-        <f t="shared" ref="J12:J52" si="10">IFERROR(I12/G12, "Not Found")</f>
+      <c r="J12" s="10">
+        <f t="shared" si="4"/>
         <v>-0.10527708280146378</v>
       </c>
       <c r="K12">
         <f t="shared" si="5"/>
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="L12">
         <v>4677800</v>
@@ -2905,13 +2930,13 @@
         <f t="shared" si="6"/>
         <v>-306086.86000000034</v>
       </c>
-      <c r="O12" s="5">
+      <c r="O12" s="10">
         <f t="shared" si="7"/>
         <v>-6.5433934755654441E-2</v>
       </c>
       <c r="P12">
         <f t="shared" si="8"/>
-        <v>39</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
@@ -2929,12 +2954,12 @@
         <v>-75511.669999999925</v>
       </c>
       <c r="E13" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-1.2912833886247806E-2</v>
       </c>
       <c r="F13">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="G13">
         <v>6223700</v>
@@ -2946,13 +2971,13 @@
         <f t="shared" si="3"/>
         <v>-314622.06000000983</v>
       </c>
-      <c r="J13" s="5">
-        <f t="shared" si="10"/>
+      <c r="J13" s="10">
+        <f t="shared" si="4"/>
         <v>-5.0552253482656594E-2</v>
       </c>
       <c r="K13">
         <f t="shared" si="5"/>
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="L13">
         <v>6207300</v>
@@ -2964,13 +2989,13 @@
         <f t="shared" si="6"/>
         <v>-150323.33000000007</v>
       </c>
-      <c r="O13" s="5">
+      <c r="O13" s="10">
         <f t="shared" si="7"/>
         <v>-2.4217184605222895E-2</v>
       </c>
       <c r="P13">
         <f t="shared" si="8"/>
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
@@ -2988,12 +3013,12 @@
         <v>-6982.6300000000047</v>
       </c>
       <c r="E14" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-1.3637949218750009E-2</v>
       </c>
       <c r="F14">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="G14">
         <v>530500</v>
@@ -3005,13 +3030,13 @@
         <f t="shared" si="3"/>
         <v>-6097.0200000000186</v>
       </c>
-      <c r="J14" s="5">
-        <f t="shared" si="10"/>
+      <c r="J14" s="10">
+        <f t="shared" si="4"/>
         <v>-1.1492968897266765E-2</v>
       </c>
       <c r="K14">
         <f t="shared" si="5"/>
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="L14">
         <v>526200</v>
@@ -3023,13 +3048,13 @@
         <f t="shared" si="6"/>
         <v>-21210.119999999995</v>
       </c>
-      <c r="O14" s="5">
+      <c r="O14" s="10">
         <f t="shared" si="7"/>
         <v>-4.0308095781071827E-2</v>
       </c>
       <c r="P14">
         <f t="shared" si="8"/>
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
@@ -3047,12 +3072,12 @@
         <v>496819.90000000596</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>3.1837408866824991E-3</v>
       </c>
       <c r="F15">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="G15">
         <v>184167800</v>
@@ -3064,13 +3089,13 @@
         <f t="shared" si="3"/>
         <v>-8201410.7500010133</v>
       </c>
-      <c r="J15" s="5">
-        <f t="shared" si="10"/>
+      <c r="J15" s="10">
+        <f t="shared" si="4"/>
         <v>-4.4532273014072019E-2</v>
       </c>
       <c r="K15">
         <f t="shared" si="5"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L15">
         <v>188953500</v>
@@ -3082,13 +3107,13 @@
         <f t="shared" si="6"/>
         <v>-4502589.1500009894</v>
       </c>
-      <c r="O15" s="5">
+      <c r="O15" s="10">
         <f t="shared" si="7"/>
         <v>-2.3829085727446114E-2</v>
       </c>
       <c r="P15">
         <f t="shared" si="8"/>
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
@@ -3106,12 +3131,12 @@
         <v>-78219.540000010282</v>
       </c>
       <c r="E16" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-1.1850188616360429E-2</v>
       </c>
       <c r="F16">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="G16">
         <v>7352500</v>
@@ -3123,13 +3148,13 @@
         <f t="shared" si="3"/>
         <v>-2035.9199999999255</v>
       </c>
-      <c r="J16" s="5">
-        <f t="shared" si="10"/>
+      <c r="J16" s="10">
+        <f t="shared" si="4"/>
         <v>-2.769017341040361E-4</v>
       </c>
       <c r="K16">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="L16">
         <v>7397200</v>
@@ -3141,13 +3166,13 @@
         <f t="shared" si="6"/>
         <v>-107</v>
       </c>
-      <c r="O16" s="5">
+      <c r="O16" s="10">
         <f t="shared" si="7"/>
         <v>-1.4464932677229222E-5</v>
       </c>
       <c r="P16">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
@@ -3165,12 +3190,12 @@
         <v>-421319.94999999925</v>
       </c>
       <c r="E17" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-2.8351094826658003E-2</v>
       </c>
       <c r="F17">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G17">
         <v>15309700</v>
@@ -3182,13 +3207,13 @@
         <f t="shared" si="3"/>
         <v>-664466.49000000022</v>
       </c>
-      <c r="J17" s="5">
-        <f t="shared" si="10"/>
+      <c r="J17" s="10">
+        <f t="shared" si="4"/>
         <v>-4.3401666263871937E-2</v>
       </c>
       <c r="K17">
         <f t="shared" si="5"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L17">
         <v>15311800</v>
@@ -3200,13 +3225,13 @@
         <f t="shared" si="6"/>
         <v>-965742.96000000089</v>
       </c>
-      <c r="O17" s="5">
+      <c r="O17" s="10">
         <f t="shared" si="7"/>
         <v>-6.3071811282801551E-2</v>
       </c>
       <c r="P17">
         <f t="shared" si="8"/>
-        <v>38</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
@@ -3224,12 +3249,12 @@
         <v>-149396.10000000987</v>
       </c>
       <c r="E18" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-5.4037002206391245E-2</v>
       </c>
       <c r="F18">
         <f t="shared" si="2"/>
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="G18">
         <v>2861000</v>
@@ -3241,13 +3266,13 @@
         <f t="shared" si="3"/>
         <v>-189254.06000000006</v>
       </c>
-      <c r="J18" s="5">
-        <f t="shared" si="10"/>
+      <c r="J18" s="10">
+        <f t="shared" si="4"/>
         <v>-6.6149619014330668E-2</v>
       </c>
       <c r="K18">
         <f t="shared" si="5"/>
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="L18">
         <v>2910600</v>
@@ -3259,13 +3284,13 @@
         <f t="shared" si="6"/>
         <v>-374962.91000000015</v>
       </c>
-      <c r="O18" s="5">
+      <c r="O18" s="10">
         <f t="shared" si="7"/>
         <v>-0.12882667147667154</v>
       </c>
       <c r="P18">
         <f t="shared" si="8"/>
-        <v>46</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
@@ -3283,12 +3308,12 @@
         <v>-376336.80000001006</v>
       </c>
       <c r="E19" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-4.258504294298146E-2</v>
       </c>
       <c r="F19">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="G19">
         <v>9713300</v>
@@ -3300,13 +3325,13 @@
         <f t="shared" si="3"/>
         <v>-721592.76000000909</v>
       </c>
-      <c r="J19" s="5">
-        <f t="shared" si="10"/>
+      <c r="J19" s="10">
+        <f t="shared" si="4"/>
         <v>-7.4289145810384635E-2</v>
       </c>
       <c r="K19">
         <f t="shared" si="5"/>
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="L19">
         <v>9343000</v>
@@ -3318,13 +3343,13 @@
         <f t="shared" si="6"/>
         <v>-576344.08999999985</v>
       </c>
-      <c r="O19" s="5">
+      <c r="O19" s="10">
         <f t="shared" si="7"/>
         <v>-6.1687262121374278E-2</v>
       </c>
       <c r="P19">
         <f t="shared" si="8"/>
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
@@ -3342,12 +3367,12 @@
         <v>-1539.8400010019541</v>
       </c>
       <c r="E20" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-1.2379538203300809E-5</v>
       </c>
       <c r="F20">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="G20">
         <v>131849400</v>
@@ -3359,13 +3384,13 @@
         <f t="shared" si="3"/>
         <v>-9775.6299999952316</v>
       </c>
-      <c r="J20" s="5">
-        <f t="shared" si="10"/>
+      <c r="J20" s="10">
+        <f t="shared" si="4"/>
         <v>-7.4142392760188761E-5</v>
       </c>
       <c r="K20">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="L20">
         <v>130621400</v>
@@ -3377,13 +3402,13 @@
         <f t="shared" si="6"/>
         <v>-116.46000100672245</v>
       </c>
-      <c r="O20" s="5">
+      <c r="O20" s="10">
         <f t="shared" si="7"/>
         <v>-8.9158438821450736E-7</v>
       </c>
       <c r="P20">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
@@ -3401,12 +3426,12 @@
         <v>-1923512.4500000998</v>
       </c>
       <c r="E21" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-7.9052463618023094E-2</v>
       </c>
       <c r="F21">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="G21">
         <v>24497400</v>
@@ -3418,13 +3443,13 @@
         <f t="shared" si="3"/>
         <v>-1841406.370000001</v>
       </c>
-      <c r="J21" s="5">
-        <f t="shared" si="10"/>
+      <c r="J21" s="10">
+        <f t="shared" si="4"/>
         <v>-7.5167420624229556E-2</v>
       </c>
       <c r="K21">
         <f t="shared" si="5"/>
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="L21">
         <v>24323000</v>
@@ -3436,13 +3461,13 @@
         <f t="shared" si="6"/>
         <v>-888926.91000010073</v>
       </c>
-      <c r="O21" s="5">
+      <c r="O21" s="10">
         <f t="shared" si="7"/>
         <v>-3.6546762734864152E-2</v>
       </c>
       <c r="P21">
         <f t="shared" si="8"/>
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
@@ -3460,12 +3485,12 @@
         <v>-153660.12000009976</v>
       </c>
       <c r="E22" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-1.3285502334437123E-2</v>
       </c>
       <c r="F22">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="G22">
         <v>11980700</v>
@@ -3477,13 +3502,13 @@
         <f t="shared" si="3"/>
         <v>-188722.03000009991</v>
       </c>
-      <c r="J22" s="5">
-        <f t="shared" si="10"/>
+      <c r="J22" s="10">
+        <f t="shared" si="4"/>
         <v>-1.5752170574348738E-2</v>
       </c>
       <c r="K22">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="L22">
         <v>11935200</v>
@@ -3495,13 +3520,13 @@
         <f t="shared" si="6"/>
         <v>-745.23000000044703</v>
       </c>
-      <c r="O22" s="5">
+      <c r="O22" s="10">
         <f t="shared" si="7"/>
         <v>-6.2439674240938325E-5</v>
       </c>
       <c r="P22">
         <f t="shared" si="8"/>
-        <v>7</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
@@ -3519,12 +3544,12 @@
         <v>-825956.59000010043</v>
       </c>
       <c r="E23" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-3.9590110100806722E-2</v>
       </c>
       <c r="F23">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="G23">
         <v>22683800</v>
@@ -3536,13 +3561,13 @@
         <f t="shared" si="3"/>
         <v>-961673.78000010177</v>
       </c>
-      <c r="J23" s="5">
-        <f t="shared" si="10"/>
+      <c r="J23" s="10">
+        <f t="shared" si="4"/>
         <v>-4.2394738976719144E-2</v>
       </c>
       <c r="K23">
         <f t="shared" si="5"/>
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="L23">
         <v>23220300</v>
@@ -3554,13 +3579,13 @@
         <f t="shared" si="6"/>
         <v>-601242.55999999866</v>
       </c>
-      <c r="O23" s="5">
+      <c r="O23" s="10">
         <f t="shared" si="7"/>
         <v>-2.5892971236375011E-2</v>
       </c>
       <c r="P23">
         <f t="shared" si="8"/>
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
@@ -3578,12 +3603,12 @@
         <v>-12230.810000000056</v>
       </c>
       <c r="E24" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-1.3334943305713101E-2</v>
       </c>
       <c r="F24">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="G24">
         <v>1112700</v>
@@ -3595,13 +3620,13 @@
         <f t="shared" si="3"/>
         <v>-45485.580000000075</v>
       </c>
-      <c r="J24" s="5">
-        <f t="shared" si="10"/>
+      <c r="J24" s="10">
+        <f t="shared" si="4"/>
         <v>-4.087856565111897E-2</v>
       </c>
       <c r="K24">
         <f t="shared" si="5"/>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="L24">
         <v>1112600</v>
@@ -3613,13 +3638,13 @@
         <f t="shared" si="6"/>
         <v>-72.879999999888241</v>
       </c>
-      <c r="O24" s="5">
+      <c r="O24" s="10">
         <f t="shared" si="7"/>
         <v>-6.5504224339284781E-5</v>
       </c>
       <c r="P24">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
@@ -3637,12 +3662,12 @@
         <v>-4950.4699999999721</v>
       </c>
       <c r="E25" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-1.0226130964676661E-2</v>
       </c>
       <c r="F25">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="G25">
         <v>505200</v>
@@ -3654,13 +3679,13 @@
         <f t="shared" si="3"/>
         <v>-8005.7900000010268</v>
       </c>
-      <c r="J25" s="5">
-        <f t="shared" si="10"/>
+      <c r="J25" s="10">
+        <f t="shared" si="4"/>
         <v>-1.5846773555029746E-2</v>
       </c>
       <c r="K25">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="L25">
         <v>496500</v>
@@ -3672,13 +3697,13 @@
         <f t="shared" si="6"/>
         <v>-1724.9000000000233</v>
       </c>
-      <c r="O25" s="5">
+      <c r="O25" s="10">
         <f t="shared" si="7"/>
         <v>-3.4741188318228064E-3</v>
       </c>
       <c r="P25">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
@@ -3696,12 +3721,12 @@
         <v>-447839.91999999993</v>
       </c>
       <c r="E26" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-8.5306091660634673E-2</v>
       </c>
       <c r="F26">
         <f t="shared" si="2"/>
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="G26">
         <v>5442200</v>
@@ -3713,13 +3738,13 @@
         <f t="shared" si="3"/>
         <v>-319870.97000000998</v>
       </c>
-      <c r="J26" s="5">
-        <f t="shared" si="10"/>
+      <c r="J26" s="10">
+        <f t="shared" si="4"/>
         <v>-5.8776040939327839E-2</v>
       </c>
       <c r="K26">
         <f t="shared" si="5"/>
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="L26">
         <v>5430700</v>
@@ -3731,13 +3756,13 @@
         <f t="shared" si="6"/>
         <v>-313464.79000000004</v>
       </c>
-      <c r="O26" s="5">
+      <c r="O26" s="10">
         <f t="shared" si="7"/>
         <v>-5.7720881286022069E-2</v>
       </c>
       <c r="P26">
         <f t="shared" si="8"/>
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
@@ -3754,13 +3779,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E27" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>Not Found</v>
-      </c>
-      <c r="F27" t="str">
+      <c r="E27" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F27">
         <f t="shared" si="2"/>
-        <v>Not Found</v>
+        <v>47</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -3772,13 +3797,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J27" s="5" t="str">
-        <f t="shared" si="10"/>
-        <v>Not Found</v>
-      </c>
-      <c r="K27" t="str">
+      <c r="J27" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>0.00%</v>
+      </c>
+      <c r="K27">
         <f t="shared" si="5"/>
-        <v>Not Found</v>
+        <v>48</v>
       </c>
       <c r="L27">
         <v>0</v>
@@ -3790,13 +3815,13 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O27" s="5" t="str">
+      <c r="O27" s="10" t="str">
         <f t="shared" si="7"/>
-        <v>Not Found</v>
-      </c>
-      <c r="P27" t="str">
+        <v>0.00%</v>
+      </c>
+      <c r="P27">
         <f t="shared" si="8"/>
-        <v>Not Found</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
@@ -3814,12 +3839,12 @@
         <v>-132457.97999999998</v>
       </c>
       <c r="E28" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-9.5782760864849215E-2</v>
       </c>
       <c r="F28">
         <f t="shared" si="2"/>
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="G28">
         <v>1545700</v>
@@ -3831,13 +3856,13 @@
         <f t="shared" si="3"/>
         <v>-264364.77</v>
       </c>
-      <c r="J28" s="5">
-        <f t="shared" si="10"/>
+      <c r="J28" s="10">
+        <f t="shared" si="4"/>
         <v>-0.17103239309050916</v>
       </c>
       <c r="K28">
         <f t="shared" si="5"/>
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="L28">
         <v>1525900</v>
@@ -3849,13 +3874,13 @@
         <f t="shared" si="6"/>
         <v>-132614.93999999994</v>
       </c>
-      <c r="O28" s="5">
+      <c r="O28" s="10">
         <f t="shared" si="7"/>
         <v>-8.6909325643882263E-2</v>
       </c>
       <c r="P28">
         <f t="shared" si="8"/>
-        <v>42</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
@@ -3873,12 +3898,12 @@
         <v>-37915.290000000037</v>
       </c>
       <c r="E29" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-1.4800253727847622E-2</v>
       </c>
       <c r="F29">
         <f t="shared" si="2"/>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G29">
         <v>2779500</v>
@@ -3890,13 +3915,13 @@
         <f t="shared" si="3"/>
         <v>-114235.56000000983</v>
       </c>
-      <c r="J29" s="5">
-        <f t="shared" si="10"/>
+      <c r="J29" s="10">
+        <f t="shared" si="4"/>
         <v>-4.1099320021590155E-2</v>
       </c>
       <c r="K29">
         <f t="shared" si="5"/>
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="L29">
         <v>2889900</v>
@@ -3908,13 +3933,13 @@
         <f t="shared" si="6"/>
         <v>-35.330000000074506</v>
       </c>
-      <c r="O29" s="5">
+      <c r="O29" s="10">
         <f t="shared" si="7"/>
         <v>-1.2225336516860273E-5</v>
       </c>
       <c r="P29">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
@@ -3932,12 +3957,12 @@
         <v>-101705.90000000037</v>
       </c>
       <c r="E30" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-8.3831374359143746E-3</v>
       </c>
       <c r="F30">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="G30">
         <v>12735900</v>
@@ -3949,13 +3974,13 @@
         <f t="shared" si="3"/>
         <v>-50385.720000099391</v>
       </c>
-      <c r="J30" s="5">
-        <f t="shared" si="10"/>
+      <c r="J30" s="10">
+        <f t="shared" si="4"/>
         <v>-3.9561962641116366E-3</v>
       </c>
       <c r="K30">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="L30">
         <v>12861300</v>
@@ -3967,13 +3992,13 @@
         <f t="shared" si="6"/>
         <v>-35290.390000000596</v>
       </c>
-      <c r="O30" s="5">
+      <c r="O30" s="10">
         <f t="shared" si="7"/>
         <v>-2.7439209100169185E-3</v>
       </c>
       <c r="P30">
         <f t="shared" si="8"/>
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
@@ -3991,12 +4016,12 @@
         <v>-24772.310000000056</v>
       </c>
       <c r="E31" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-1.4030533529678329E-2</v>
       </c>
       <c r="F31">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="G31">
         <v>1823300</v>
@@ -4008,13 +4033,13 @@
         <f t="shared" si="3"/>
         <v>-60623.149999999907</v>
       </c>
-      <c r="J31" s="5">
-        <f t="shared" si="10"/>
+      <c r="J31" s="10">
+        <f t="shared" si="4"/>
         <v>-3.3249136181648611E-2</v>
       </c>
       <c r="K31">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="L31">
         <v>1870700</v>
@@ -4026,13 +4051,13 @@
         <f t="shared" si="6"/>
         <v>-69308.659999999916</v>
       </c>
-      <c r="O31" s="5">
+      <c r="O31" s="10">
         <f t="shared" si="7"/>
         <v>-3.7049585716576634E-2</v>
       </c>
       <c r="P31">
         <f t="shared" si="8"/>
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
@@ -4050,12 +4075,12 @@
         <v>-73762.280000009574</v>
       </c>
       <c r="E32" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-1.2294942827617691E-2</v>
       </c>
       <c r="F32">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="G32">
         <v>6195500</v>
@@ -4067,13 +4092,13 @@
         <f t="shared" si="3"/>
         <v>-110514.53000000026</v>
       </c>
-      <c r="J32" s="5">
-        <f t="shared" si="10"/>
+      <c r="J32" s="10">
+        <f t="shared" si="4"/>
         <v>-1.7837871035428981E-2</v>
       </c>
       <c r="K32">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="L32">
         <v>6157400</v>
@@ -4085,13 +4110,13 @@
         <f t="shared" si="6"/>
         <v>-169827.98000000045</v>
       </c>
-      <c r="O32" s="5">
+      <c r="O32" s="10">
         <f t="shared" si="7"/>
         <v>-2.7581118653977402E-2</v>
       </c>
       <c r="P32">
         <f t="shared" si="8"/>
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
@@ -4109,12 +4134,12 @@
         <v>-7418835.2699990273</v>
       </c>
       <c r="E33" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-7.9969930789269058E-3</v>
       </c>
       <c r="F33">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G33">
         <v>979671000</v>
@@ -4126,13 +4151,13 @@
         <f t="shared" si="3"/>
         <v>-2602486.5199999809</v>
       </c>
-      <c r="J33" s="5">
-        <f t="shared" si="10"/>
+      <c r="J33" s="10">
+        <f t="shared" si="4"/>
         <v>-2.6564903115433454E-3</v>
       </c>
       <c r="K33">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="L33">
         <v>989572899.99999905</v>
@@ -4144,13 +4169,13 @@
         <f t="shared" si="6"/>
         <v>-5456610.5900000334</v>
       </c>
-      <c r="O33" s="5">
+      <c r="O33" s="10">
         <f t="shared" si="7"/>
         <v>-5.5141067323084929E-3</v>
       </c>
       <c r="P33">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
@@ -4168,12 +4193,12 @@
         <v>-79341.779999999795</v>
       </c>
       <c r="E34" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-1.8939149738619768E-2</v>
       </c>
       <c r="F34">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G34">
         <v>4350600</v>
@@ -4185,13 +4210,13 @@
         <f t="shared" si="3"/>
         <v>-213011.23000001023</v>
       </c>
-      <c r="J34" s="5">
-        <f t="shared" si="10"/>
+      <c r="J34" s="10">
+        <f t="shared" si="4"/>
         <v>-4.8961345561534093E-2</v>
       </c>
       <c r="K34">
         <f t="shared" si="5"/>
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="L34">
         <v>4345600</v>
@@ -4203,13 +4228,13 @@
         <f t="shared" si="6"/>
         <v>-115798.49000000022</v>
       </c>
-      <c r="O34" s="5">
+      <c r="O34" s="10">
         <f t="shared" si="7"/>
         <v>-2.6647296115611244E-2</v>
       </c>
       <c r="P34">
         <f t="shared" si="8"/>
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
@@ -4226,13 +4251,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E35" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>Not Found</v>
-      </c>
-      <c r="F35" t="str">
+      <c r="E35" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F35">
         <f t="shared" si="2"/>
-        <v>Not Found</v>
+        <v>47</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -4244,13 +4269,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J35" s="5" t="str">
-        <f t="shared" si="10"/>
-        <v>Not Found</v>
-      </c>
-      <c r="K35" t="str">
+      <c r="J35" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>0.00%</v>
+      </c>
+      <c r="K35">
         <f t="shared" si="5"/>
-        <v>Not Found</v>
+        <v>48</v>
       </c>
       <c r="L35">
         <v>0</v>
@@ -4262,13 +4287,13 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O35" s="5" t="str">
+      <c r="O35" s="10" t="str">
         <f t="shared" si="7"/>
-        <v>Not Found</v>
-      </c>
-      <c r="P35" t="str">
+        <v>0.00%</v>
+      </c>
+      <c r="P35">
         <f t="shared" si="8"/>
-        <v>Not Found</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
@@ -4286,12 +4311,12 @@
         <v>-62776.72000000102</v>
       </c>
       <c r="E36" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-7.8647857679780775E-2</v>
       </c>
       <c r="F36">
         <f t="shared" si="2"/>
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="G36">
         <v>898700</v>
@@ -4303,13 +4328,13 @@
         <f t="shared" si="3"/>
         <v>-157733.05000000098</v>
       </c>
-      <c r="J36" s="5">
-        <f t="shared" si="10"/>
+      <c r="J36" s="10">
+        <f t="shared" si="4"/>
         <v>-0.17551246244575608</v>
       </c>
       <c r="K36">
         <f t="shared" si="5"/>
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="L36">
         <v>878300</v>
@@ -4321,13 +4346,13 @@
         <f t="shared" si="6"/>
         <v>-101084.71000000101</v>
       </c>
-      <c r="O36" s="5">
+      <c r="O36" s="10">
         <f t="shared" si="7"/>
         <v>-0.11509132414892521</v>
       </c>
       <c r="P36">
         <f t="shared" si="8"/>
-        <v>44</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
@@ -4345,12 +4370,12 @@
         <v>-82352.260000010021</v>
       </c>
       <c r="E37" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-3.9444515758219188E-2</v>
       </c>
       <c r="F37">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="G37">
         <v>2229200</v>
@@ -4362,13 +4387,13 @@
         <f t="shared" si="3"/>
         <v>-110256.79000000004</v>
       </c>
-      <c r="J37" s="5">
-        <f t="shared" si="10"/>
+      <c r="J37" s="10">
+        <f t="shared" si="4"/>
         <v>-4.9460250314014013E-2</v>
       </c>
       <c r="K37">
         <f t="shared" si="5"/>
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L37">
         <v>2296900</v>
@@ -4380,13 +4405,13 @@
         <f t="shared" si="6"/>
         <v>-188181.66000000015</v>
       </c>
-      <c r="O37" s="5">
+      <c r="O37" s="10">
         <f t="shared" si="7"/>
         <v>-8.1928538464887526E-2</v>
       </c>
       <c r="P37">
         <f t="shared" si="8"/>
-        <v>41</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
@@ -4404,12 +4429,12 @@
         <v>-16630.180000000051</v>
       </c>
       <c r="E38" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-1.9443680579913542E-2</v>
       </c>
       <c r="F38">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G38">
         <v>792800</v>
@@ -4421,13 +4446,13 @@
         <f t="shared" si="3"/>
         <v>-39348.040000000037</v>
       </c>
-      <c r="J38" s="5">
-        <f t="shared" si="10"/>
+      <c r="J38" s="10">
+        <f t="shared" si="4"/>
         <v>-4.9631735620585316E-2</v>
       </c>
       <c r="K38">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="L38">
         <v>777800</v>
@@ -4439,13 +4464,13 @@
         <f t="shared" si="6"/>
         <v>-136.73999999999069</v>
       </c>
-      <c r="O38" s="5">
+      <c r="O38" s="10">
         <f t="shared" si="7"/>
         <v>-1.7580354847003174E-4</v>
       </c>
       <c r="P38">
         <f t="shared" si="8"/>
-        <v>9</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
@@ -4463,12 +4488,12 @@
         <v>-70791.13</v>
       </c>
       <c r="E39" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-8.008952370177623E-2</v>
       </c>
       <c r="F39">
         <f t="shared" si="2"/>
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="G39">
         <v>1294400</v>
@@ -4480,13 +4505,13 @@
         <f t="shared" si="3"/>
         <v>-180157.72000000998</v>
       </c>
-      <c r="J39" s="5">
-        <f t="shared" si="10"/>
+      <c r="J39" s="10">
+        <f t="shared" si="4"/>
         <v>-0.13918241656366656</v>
       </c>
       <c r="K39">
         <f t="shared" si="5"/>
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="L39">
         <v>1759500</v>
@@ -4498,13 +4523,13 @@
         <f t="shared" si="6"/>
         <v>-79036.1300000099</v>
       </c>
-      <c r="O39" s="5">
+      <c r="O39" s="10">
         <f t="shared" si="7"/>
         <v>-4.4919653310605226E-2</v>
       </c>
       <c r="P39">
         <f t="shared" si="8"/>
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
@@ -4522,12 +4547,12 @@
         <v>-816758.14000009745</v>
       </c>
       <c r="E40" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-2.1279773539092578E-2</v>
       </c>
       <c r="F40">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G40">
         <v>39964900</v>
@@ -4539,13 +4564,13 @@
         <f t="shared" si="3"/>
         <v>-1869659.8100000992</v>
       </c>
-      <c r="J40" s="5">
-        <f t="shared" si="10"/>
+      <c r="J40" s="10">
+        <f t="shared" si="4"/>
         <v>-4.6782546934937892E-2</v>
       </c>
       <c r="K40">
         <f t="shared" si="5"/>
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="L40">
         <v>40216700</v>
@@ -4557,13 +4582,13 @@
         <f t="shared" si="6"/>
         <v>-610436.29000010341</v>
       </c>
-      <c r="O40" s="5">
+      <c r="O40" s="10">
         <f t="shared" si="7"/>
         <v>-1.5178676768608648E-2</v>
       </c>
       <c r="P40">
         <f t="shared" si="8"/>
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
@@ -4581,12 +4606,12 @@
         <v>-184239.79000001028</v>
       </c>
       <c r="E41" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-4.0110550149132493E-2</v>
       </c>
       <c r="F41">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="G41">
         <v>5089500</v>
@@ -4598,13 +4623,13 @@
         <f t="shared" si="3"/>
         <v>-133456.33000001032</v>
       </c>
-      <c r="J41" s="5">
-        <f t="shared" si="10"/>
+      <c r="J41" s="10">
+        <f t="shared" si="4"/>
         <v>-2.6221894095689226E-2</v>
       </c>
       <c r="K41">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="L41">
         <v>4799900</v>
@@ -4616,13 +4641,13 @@
         <f t="shared" si="6"/>
         <v>-82077.349999999627</v>
       </c>
-      <c r="O41" s="5">
+      <c r="O41" s="10">
         <f t="shared" si="7"/>
         <v>-1.7099804162586642E-2</v>
       </c>
       <c r="P41">
         <f t="shared" si="8"/>
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
@@ -4640,12 +4665,12 @@
         <v>-41624.320001006126</v>
       </c>
       <c r="E42" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-2.2070943135841053E-4</v>
       </c>
       <c r="F42">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="G42">
         <v>199130300</v>
@@ -4657,13 +4682,13 @@
         <f t="shared" si="3"/>
         <v>-2375266.6899999976</v>
       </c>
-      <c r="J42" s="5">
-        <f t="shared" si="10"/>
+      <c r="J42" s="10">
+        <f t="shared" si="4"/>
         <v>-1.1928203241796942E-2</v>
       </c>
       <c r="K42">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="L42">
         <v>199954600</v>
@@ -4675,13 +4700,13 @@
         <f t="shared" si="6"/>
         <v>-36.250001013278961</v>
       </c>
-      <c r="O42" s="5">
+      <c r="O42" s="10">
         <f t="shared" si="7"/>
         <v>-1.8129115815929696E-7</v>
       </c>
       <c r="P42">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
@@ -4699,12 +4724,12 @@
         <v>-166754.16999999993</v>
       </c>
       <c r="E43" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-2.0497353541313264E-2</v>
       </c>
       <c r="F43">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G43">
         <v>8560800</v>
@@ -4716,13 +4741,13 @@
         <f t="shared" si="3"/>
         <v>-389327.98000000045</v>
       </c>
-      <c r="J43" s="5">
-        <f t="shared" si="10"/>
+      <c r="J43" s="10">
+        <f t="shared" si="4"/>
         <v>-4.5477990374731388E-2</v>
       </c>
       <c r="K43">
         <f t="shared" si="5"/>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="L43">
         <v>8497500</v>
@@ -4734,13 +4759,13 @@
         <f t="shared" si="6"/>
         <v>-346517.43000000995</v>
       </c>
-      <c r="O43" s="5">
+      <c r="O43" s="10">
         <f t="shared" si="7"/>
         <v>-4.0778750220654303E-2</v>
       </c>
       <c r="P43">
         <f t="shared" si="8"/>
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
@@ -4758,12 +4783,12 @@
         <v>-294095.62000000104</v>
       </c>
       <c r="E44" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-9.7760750186150751E-3</v>
       </c>
       <c r="F44">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="G44">
         <v>31040700</v>
@@ -4775,13 +4800,13 @@
         <f t="shared" si="3"/>
         <v>-246988.51999999955</v>
       </c>
-      <c r="J44" s="5">
-        <f t="shared" si="10"/>
+      <c r="J44" s="10">
+        <f t="shared" si="4"/>
         <v>-7.9569249404813532E-3</v>
       </c>
       <c r="K44">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="L44">
         <v>31282200</v>
@@ -4793,13 +4818,13 @@
         <f t="shared" si="6"/>
         <v>-58.75</v>
       </c>
-      <c r="O44" s="5">
+      <c r="O44" s="10">
         <f t="shared" si="7"/>
         <v>-1.8780648419868168E-6</v>
       </c>
       <c r="P44">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
@@ -4817,12 +4842,12 @@
         <v>-712015.95000009984</v>
       </c>
       <c r="E45" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-1.287514194887851E-2</v>
       </c>
       <c r="F45">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="G45">
         <v>56792200</v>
@@ -4834,13 +4859,13 @@
         <f t="shared" si="3"/>
         <v>-2197246.0400001034</v>
       </c>
-      <c r="J45" s="5">
-        <f t="shared" si="10"/>
+      <c r="J45" s="10">
+        <f t="shared" si="4"/>
         <v>-3.8689222111488959E-2</v>
       </c>
       <c r="K45">
         <f t="shared" si="5"/>
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="L45">
         <v>56027100</v>
@@ -4852,13 +4877,13 @@
         <f t="shared" si="6"/>
         <v>-640550.34000010043</v>
       </c>
-      <c r="O45" s="5">
+      <c r="O45" s="10">
         <f t="shared" si="7"/>
         <v>-1.1432866237947358E-2</v>
       </c>
       <c r="P45">
         <f t="shared" si="8"/>
-        <v>17</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
@@ -4876,12 +4901,12 @@
         <v>-777.57000000000698</v>
       </c>
       <c r="E46" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-3.0010420686993711E-3</v>
       </c>
       <c r="F46">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="G46">
         <v>266000</v>
@@ -4893,13 +4918,13 @@
         <f t="shared" si="3"/>
         <v>-8597.090000000986</v>
       </c>
-      <c r="J46" s="5">
-        <f t="shared" si="10"/>
+      <c r="J46" s="10">
+        <f t="shared" si="4"/>
         <v>-3.2319887218048821E-2</v>
       </c>
       <c r="K46">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="L46">
         <v>267100</v>
@@ -4911,13 +4936,13 @@
         <f t="shared" si="6"/>
         <v>-12346.840000000986</v>
       </c>
-      <c r="O46" s="5">
+      <c r="O46" s="10">
         <f t="shared" si="7"/>
         <v>-4.6225533508053113E-2</v>
       </c>
       <c r="P46">
         <f t="shared" si="8"/>
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
@@ -4935,12 +4960,12 @@
         <v>-12273.280000001192</v>
       </c>
       <c r="E47" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-1.7435939690898361E-4</v>
       </c>
       <c r="F47">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="G47">
         <v>73467000</v>
@@ -4952,13 +4977,13 @@
         <f t="shared" si="3"/>
         <v>-24458.340000003576</v>
       </c>
-      <c r="J47" s="5">
-        <f t="shared" si="10"/>
+      <c r="J47" s="10">
+        <f t="shared" si="4"/>
         <v>-3.3291600310348285E-4</v>
       </c>
       <c r="K47">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="L47">
         <v>75072800</v>
@@ -4970,13 +4995,13 @@
         <f t="shared" si="6"/>
         <v>-21970.820000097156</v>
       </c>
-      <c r="O47" s="5">
+      <c r="O47" s="10">
         <f t="shared" si="7"/>
         <v>-2.9266019117572752E-4</v>
       </c>
       <c r="P47">
         <f t="shared" si="8"/>
-        <v>11</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
@@ -4994,12 +5019,12 @@
         <v>-209747.43000000995</v>
       </c>
       <c r="E48" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-3.1133192323107857E-2</v>
       </c>
       <c r="F48">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G48">
         <v>7214700</v>
@@ -5011,13 +5036,13 @@
         <f t="shared" si="3"/>
         <v>-292627.44000000041</v>
       </c>
-      <c r="J48" s="5">
-        <f t="shared" si="10"/>
+      <c r="J48" s="10">
+        <f t="shared" si="4"/>
         <v>-4.0559890224125802E-2</v>
       </c>
       <c r="K48">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="L48">
         <v>7289800</v>
@@ -5029,13 +5054,13 @@
         <f t="shared" si="6"/>
         <v>-407449.76000001002</v>
       </c>
-      <c r="O48" s="5">
+      <c r="O48" s="10">
         <f t="shared" si="7"/>
         <v>-5.5893132870587676E-2</v>
       </c>
       <c r="P48">
         <f t="shared" si="8"/>
-        <v>34</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.3">
@@ -5053,12 +5078,12 @@
         <v>-1700.570000000007</v>
       </c>
       <c r="E49" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-1.8444360086767971E-2</v>
       </c>
       <c r="F49">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="G49">
         <v>102600</v>
@@ -5070,13 +5095,13 @@
         <f t="shared" si="3"/>
         <v>-7133.1199999999953</v>
       </c>
-      <c r="J49" s="5">
-        <f t="shared" si="10"/>
+      <c r="J49" s="10">
+        <f t="shared" si="4"/>
         <v>-6.9523586744639335E-2</v>
       </c>
       <c r="K49">
         <f t="shared" si="5"/>
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="L49">
         <v>0</v>
@@ -5088,13 +5113,13 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O49" s="5" t="str">
+      <c r="O49" s="10" t="str">
         <f t="shared" si="7"/>
-        <v>Not Found</v>
-      </c>
-      <c r="P49" t="str">
+        <v>0.00%</v>
+      </c>
+      <c r="P49">
         <f t="shared" si="8"/>
-        <v>Not Found</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.3">
@@ -5112,12 +5137,12 @@
         <v>0</v>
       </c>
       <c r="E50" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F50">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="G50">
         <v>859100</v>
@@ -5129,13 +5154,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J50" s="5">
-        <f t="shared" si="10"/>
+      <c r="J50" s="10">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K50">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="L50">
         <v>843200</v>
@@ -5147,13 +5172,13 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O50" s="5">
+      <c r="O50" s="10">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P50">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.3">
@@ -5171,12 +5196,12 @@
         <v>-110074.66000000946</v>
       </c>
       <c r="E51" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-1.2785255822058129E-2</v>
       </c>
       <c r="F51">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="G51">
         <v>8925500</v>
@@ -5188,13 +5213,13 @@
         <f t="shared" si="3"/>
         <v>-326440.38000000082</v>
       </c>
-      <c r="J51" s="5">
-        <f t="shared" si="10"/>
+      <c r="J51" s="10">
+        <f t="shared" si="4"/>
         <v>-3.6573903982970231E-2</v>
       </c>
       <c r="K51">
         <f t="shared" si="5"/>
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="L51">
         <v>8833900</v>
@@ -5206,13 +5231,13 @@
         <f t="shared" si="6"/>
         <v>-98056.689999999478</v>
       </c>
-      <c r="O51" s="5">
+      <c r="O51" s="10">
         <f t="shared" si="7"/>
         <v>-1.1100045280114048E-2</v>
       </c>
       <c r="P51">
         <f t="shared" si="8"/>
-        <v>16</v>
+        <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.3">
@@ -5230,12 +5255,12 @@
         <v>-196315.20000000019</v>
       </c>
       <c r="E52" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-8.009596083231342E-2</v>
       </c>
       <c r="F52">
         <f t="shared" si="2"/>
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="G52">
         <v>2440700</v>
@@ -5247,13 +5272,13 @@
         <f t="shared" si="3"/>
         <v>-236027.12000000011</v>
       </c>
-      <c r="J52" s="5">
-        <f t="shared" si="10"/>
+      <c r="J52" s="10">
+        <f t="shared" si="4"/>
         <v>-9.6704683082722218E-2</v>
       </c>
       <c r="K52">
         <f t="shared" si="5"/>
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="L52">
         <v>2321600</v>
@@ -5265,13 +5290,13 @@
         <f t="shared" si="6"/>
         <v>-264764.74</v>
       </c>
-      <c r="O52" s="5">
+      <c r="O52" s="10">
         <f t="shared" si="7"/>
         <v>-0.11404408166781529</v>
       </c>
       <c r="P52">
         <f t="shared" si="8"/>
-        <v>43</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.3">
@@ -5305,11 +5330,11 @@
         <v>-36209.630000000005</v>
       </c>
       <c r="C56">
-        <f t="shared" ref="C56:D61" si="11">VLOOKUP($A56,$A$1:$P$52,MATCH(C$55,$A$1:$P$1,0))</f>
+        <f t="shared" ref="C56:D56" si="9">VLOOKUP($A56,$A$1:$P$52,MATCH(C$55,$A$1:$P$1,0))</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D56">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -5318,11 +5343,11 @@
         <v>25</v>
       </c>
       <c r="B57">
-        <f t="shared" ref="B57:B61" si="12">VLOOKUP($A57,$A$1:$P$52,MATCH(B$55,$A$1:$P$1,0))</f>
+        <f t="shared" ref="B57:B61" si="10">VLOOKUP($A57,$A$1:$P$52,MATCH(B$55,$A$1:$P$1,0))</f>
         <v>0</v>
       </c>
       <c r="C57">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="C56:D61" si="11">VLOOKUP($A57,$A$1:$P$52,MATCH(C$55,$A$1:$P$1,0))</f>
         <v>0</v>
       </c>
       <c r="D57">
@@ -5335,7 +5360,7 @@
         <v>32</v>
       </c>
       <c r="B58">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C58">
@@ -5352,7 +5377,7 @@
         <v>38</v>
       </c>
       <c r="B59">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C59">
@@ -5369,7 +5394,7 @@
         <v>39</v>
       </c>
       <c r="B60">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C60">
@@ -5386,7 +5411,7 @@
         <v>55</v>
       </c>
       <c r="B61">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C61">
@@ -5417,230 +5442,226 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>24</v>
       </c>
-      <c r="B65">
-        <f>_xlfn.XLOOKUP(A65,$A$1:$A$52,$D$1:$D$52)</f>
+      <c r="B65" cm="1">
+        <f t="array" ref="B65">_xlfn.XLOOKUP($A65,$A$2:$A$52,INDEX($A$2:$P$52,,MATCH(B$64,$A$1:$P$1,0)))</f>
         <v>-36209.630000000005</v>
       </c>
-      <c r="C65">
-        <f>_xlfn.XLOOKUP(A65,$A$1:$A$52,$I$1:$I$52)</f>
+      <c r="C65" cm="1">
+        <f t="array" ref="C65">_xlfn.XLOOKUP($A65,$A$2:$A$52,INDEX($A$2:$P$52,,MATCH(C$64,$A$1:$P$1,0)))</f>
         <v>-27292.159999999974</v>
       </c>
-      <c r="D65">
-        <f>_xlfn.XLOOKUP(A65,$A$1:$A$52,$N$1:$N$52)</f>
+      <c r="D65" cm="1">
+        <f t="array" ref="D65">_xlfn.XLOOKUP($A65,$A$2:$A$52,INDEX($A$2:$P$52,,MATCH(D$64,$A$1:$P$1,0)))</f>
         <v>-9181.0800000000163</v>
       </c>
-      <c r="E65" t="e">
-        <f>_xlfn.XLOOKUP(A65,A2:A52,MATCH(B64,A1:P1,0))</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>25</v>
       </c>
-      <c r="B66">
-        <f t="shared" ref="B66:B70" si="13">_xlfn.XLOOKUP(A66,$A$1:$A$52,$D$1:$D$52)</f>
+      <c r="B66" cm="1">
+        <f t="array" ref="B66">_xlfn.XLOOKUP($A66,$A$2:$A$52,INDEX($A$2:$P$52,,MATCH(B$64,$A$1:$P$1,0)))</f>
         <v>0</v>
       </c>
-      <c r="C66">
-        <f t="shared" ref="C66:C70" si="14">_xlfn.XLOOKUP(A66,$A$1:$A$52,$I$1:$I$52)</f>
+      <c r="C66" cm="1">
+        <f t="array" ref="C66">_xlfn.XLOOKUP($A66,$A$2:$A$52,INDEX($A$2:$P$52,,MATCH(C$64,$A$1:$P$1,0)))</f>
         <v>0</v>
       </c>
-      <c r="D66">
-        <f t="shared" ref="D66:D70" si="15">_xlfn.XLOOKUP(A66,$A$1:$A$52,$N$1:$N$52)</f>
+      <c r="D66" cm="1">
+        <f t="array" ref="D66">_xlfn.XLOOKUP($A66,$A$2:$A$52,INDEX($A$2:$P$52,,MATCH(D$64,$A$1:$P$1,0)))</f>
         <v>-311228.08999999997</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>32</v>
       </c>
-      <c r="B67">
+      <c r="B67" cm="1">
+        <f t="array" ref="B67">_xlfn.XLOOKUP($A67,$A$2:$A$52,INDEX($A$2:$P$52,,MATCH(B$64,$A$1:$P$1,0)))</f>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C67" cm="1">
+        <f t="array" ref="C67">_xlfn.XLOOKUP($A67,$A$2:$A$52,INDEX($A$2:$P$52,,MATCH(C$64,$A$1:$P$1,0)))</f>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="D67" cm="1">
+        <f t="array" ref="D67">_xlfn.XLOOKUP($A67,$A$2:$A$52,INDEX($A$2:$P$52,,MATCH(D$64,$A$1:$P$1,0)))</f>
+        <v>-374962.91000000015</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>38</v>
+      </c>
+      <c r="B68" cm="1">
+        <f t="array" ref="B68">_xlfn.XLOOKUP($A68,$A$2:$A$52,INDEX($A$2:$P$52,,MATCH(B$64,$A$1:$P$1,0)))</f>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C68" cm="1">
+        <f t="array" ref="C68">_xlfn.XLOOKUP($A68,$A$2:$A$52,INDEX($A$2:$P$52,,MATCH(C$64,$A$1:$P$1,0)))</f>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="D68" cm="1">
+        <f t="array" ref="D68">_xlfn.XLOOKUP($A68,$A$2:$A$52,INDEX($A$2:$P$52,,MATCH(D$64,$A$1:$P$1,0)))</f>
+        <v>-72.879999999888241</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>39</v>
+      </c>
+      <c r="B69" cm="1">
+        <f t="array" ref="B69">_xlfn.XLOOKUP($A69,$A$2:$A$52,INDEX($A$2:$P$52,,MATCH(B$64,$A$1:$P$1,0)))</f>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C69" cm="1">
+        <f t="array" ref="C69">_xlfn.XLOOKUP($A69,$A$2:$A$52,INDEX($A$2:$P$52,,MATCH(C$64,$A$1:$P$1,0)))</f>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D69" cm="1">
+        <f t="array" ref="D69">_xlfn.XLOOKUP($A69,$A$2:$A$52,INDEX($A$2:$P$52,,MATCH(D$64,$A$1:$P$1,0)))</f>
+        <v>-1724.9000000000233</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>55</v>
+      </c>
+      <c r="B70" cm="1">
+        <f t="array" ref="B70">_xlfn.XLOOKUP($A70,$A$2:$A$52,INDEX($A$2:$P$52,,MATCH(B$64,$A$1:$P$1,0)))</f>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C70" cm="1">
+        <f t="array" ref="C70">_xlfn.XLOOKUP($A70,$A$2:$A$52,INDEX($A$2:$P$52,,MATCH(C$64,$A$1:$P$1,0)))</f>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="D70" cm="1">
+        <f t="array" ref="D70">_xlfn.XLOOKUP($A70,$A$2:$A$52,INDEX($A$2:$P$52,,MATCH(D$64,$A$1:$P$1,0)))</f>
+        <v>-82077.349999999627</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>24</v>
+      </c>
+      <c r="B74">
+        <f>INDEX($A$2:$P$52, MATCH($A74,$A$2:$A$52,0),MATCH(B$73,$A$1:$P$1,0))</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="C74">
+        <f t="shared" ref="C74:D79" si="12">INDEX($A$2:$P$52, MATCH($A74,$A$2:$A$52,0),MATCH(C$73,$A$1:$P$1,0))</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="12"/>
+        <v>-9181.0800000000163</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>25</v>
+      </c>
+      <c r="B75">
+        <f t="shared" ref="B75:B79" si="13">INDEX($A$2:$P$52, MATCH($A75,$A$2:$A$52,0),MATCH(B$73,$A$1:$P$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="12"/>
+        <v>-311228.08999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>32</v>
+      </c>
+      <c r="B76">
         <f t="shared" si="13"/>
         <v>-149396.10000000987</v>
       </c>
-      <c r="C67">
-        <f t="shared" si="14"/>
+      <c r="C76">
+        <f t="shared" si="12"/>
         <v>-189254.06000000006</v>
       </c>
-      <c r="D67">
-        <f t="shared" si="15"/>
+      <c r="D76">
+        <f t="shared" si="12"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>38</v>
       </c>
-      <c r="B68">
+      <c r="B77">
         <f t="shared" si="13"/>
         <v>-12230.810000000056</v>
       </c>
-      <c r="C68">
-        <f t="shared" si="14"/>
+      <c r="C77">
+        <f t="shared" si="12"/>
         <v>-45485.580000000075</v>
       </c>
-      <c r="D68">
-        <f t="shared" si="15"/>
+      <c r="D77">
+        <f t="shared" si="12"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>39</v>
       </c>
-      <c r="B69">
+      <c r="B78">
         <f t="shared" si="13"/>
         <v>-4950.4699999999721</v>
       </c>
-      <c r="C69">
-        <f t="shared" si="14"/>
+      <c r="C78">
+        <f t="shared" si="12"/>
         <v>-8005.7900000010268</v>
       </c>
-      <c r="D69">
-        <f t="shared" si="15"/>
+      <c r="D78">
+        <f t="shared" si="12"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>55</v>
       </c>
-      <c r="B70">
+      <c r="B79">
         <f t="shared" si="13"/>
         <v>-184239.79000001028</v>
       </c>
-      <c r="C70">
-        <f t="shared" si="14"/>
+      <c r="C79">
+        <f t="shared" si="12"/>
         <v>-133456.33000001032</v>
       </c>
-      <c r="D70">
-        <f t="shared" si="15"/>
-        <v>-82077.349999999627</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>24</v>
-      </c>
-      <c r="B74">
-        <f>INDEX($D$1:$D$52,MATCH(A74,$A$1:$A$52,0))</f>
-        <v>-36209.630000000005</v>
-      </c>
-      <c r="C74">
-        <f>INDEX($I$1:$I$52,MATCH(A74,$A$1:$A$52,0))</f>
-        <v>-27292.159999999974</v>
-      </c>
-      <c r="D74">
-        <f>INDEX($N$1:$N$52,MATCH(A74,$A$1:$A$52,0))</f>
-        <v>-9181.0800000000163</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>25</v>
-      </c>
-      <c r="B75">
-        <f t="shared" ref="B75:B79" si="16">INDEX($D$1:$D$52,MATCH(A75,$A$1:$A$52,0))</f>
-        <v>0</v>
-      </c>
-      <c r="C75">
-        <f t="shared" ref="C75:C79" si="17">INDEX($I$1:$I$52,MATCH(A75,$A$1:$A$52,0))</f>
-        <v>0</v>
-      </c>
-      <c r="D75">
-        <f t="shared" ref="D75:D79" si="18">INDEX($N$1:$N$52,MATCH(A75,$A$1:$A$52,0))</f>
-        <v>-311228.08999999997</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>32</v>
-      </c>
-      <c r="B76">
-        <f t="shared" si="16"/>
-        <v>-149396.10000000987</v>
-      </c>
-      <c r="C76">
-        <f t="shared" si="17"/>
-        <v>-189254.06000000006</v>
-      </c>
-      <c r="D76">
-        <f t="shared" si="18"/>
-        <v>-374962.91000000015</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>38</v>
-      </c>
-      <c r="B77">
-        <f t="shared" si="16"/>
-        <v>-12230.810000000056</v>
-      </c>
-      <c r="C77">
-        <f t="shared" si="17"/>
-        <v>-45485.580000000075</v>
-      </c>
-      <c r="D77">
-        <f t="shared" si="18"/>
-        <v>-72.879999999888241</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>39</v>
-      </c>
-      <c r="B78">
-        <f t="shared" si="16"/>
-        <v>-4950.4699999999721</v>
-      </c>
-      <c r="C78">
-        <f t="shared" si="17"/>
-        <v>-8005.7900000010268</v>
-      </c>
-      <c r="D78">
-        <f t="shared" si="18"/>
-        <v>-1724.9000000000233</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>55</v>
-      </c>
-      <c r="B79">
-        <f t="shared" si="16"/>
-        <v>-184239.79000001028</v>
-      </c>
-      <c r="C79">
-        <f t="shared" si="17"/>
-        <v>-133456.33000001032</v>
-      </c>
       <c r="D79">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -5749,25 +5770,88 @@
       <c r="A91" t="s">
         <v>73</v>
       </c>
-      <c r="C91" s="5"/>
-      <c r="E91" s="5"/>
-      <c r="G91" s="5"/>
+      <c r="B91" t="str" cm="1">
+        <f t="array" ref="B91">_xlfn.XLOOKUP($B$89,INDEX($A$2:$P$52,,MATCH( A91&amp;"_rank",$A$1:$P$1,0)),$A$2:$A$52)</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="C91" s="5" cm="1">
+        <f t="array" ref="C91">_xlfn.XLOOKUP($B$89,INDEX($A$2:$P$52,,MATCH( A91&amp;"_rank",$A$1:$P$1,0)),INDEX($A$2:$P$52,,MATCH(A91&amp;"_diff_pct",$A$1:$P$1,0)))</f>
+        <v>-0.15235918433091292</v>
+      </c>
+      <c r="D91" t="str" cm="1">
+        <f t="array" ref="D91">_xlfn.XLOOKUP($D$89,INDEX($A$2:$P$52,,MATCH( A91&amp;"_rank",$A$1:$P$1,0)),$A$2:$A$52)</f>
+        <v>Circuit Court Clerk</v>
+      </c>
+      <c r="E91" s="5" cm="1">
+        <f t="array" ref="E91">_xlfn.XLOOKUP($D$89,INDEX($A$2:$P$52,,MATCH( A91&amp;"_rank",$A$1:$P$1,0)),INDEX($A$2:$P$52,,MATCH(A91&amp;"_diff_pct",$A$1:$P$1,0)))</f>
+        <v>-0.11502817362571344</v>
+      </c>
+      <c r="F91" t="str" cm="1">
+        <f t="array" ref="F91">_xlfn.XLOOKUP($F$89,INDEX($A$2:$P$52,,MATCH( A91&amp;"_rank",$A$1:$P$1,0)),$A$2:$A$52)</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="G91" s="5" cm="1">
+        <f t="array" ref="G91">_xlfn.XLOOKUP($F$89,INDEX($A$2:$P$52,,MATCH( A91&amp;"_rank",$A$1:$P$1,0)),INDEX($A$2:$P$52,,MATCH(A91&amp;"_diff_pct",$A$1:$P$1,0)))</f>
+        <v>-9.5782760864849215E-2</v>
+      </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>74</v>
       </c>
-      <c r="C92" s="5"/>
-      <c r="E92" s="5"/>
-      <c r="G92" s="5"/>
+      <c r="B92" t="str" cm="1">
+        <f t="array" ref="B92">_xlfn.XLOOKUP($B$89,INDEX($A$2:$P$52,,MATCH( A92&amp;"_rank",$A$1:$P$1,0)),$A$2:$A$52)</f>
+        <v>Metropolitan Clerk</v>
+      </c>
+      <c r="C92" s="5" cm="1">
+        <f t="array" ref="C92">_xlfn.XLOOKUP($B$89,INDEX($A$2:$P$52,,MATCH( A92&amp;"_rank",$A$1:$P$1,0)),INDEX($A$2:$P$52,,MATCH(A92&amp;"_diff_pct",$A$1:$P$1,0)))</f>
+        <v>-0.17551246244575608</v>
+      </c>
+      <c r="D92" t="str" cm="1">
+        <f t="array" ref="D92">_xlfn.XLOOKUP($D$89,INDEX($A$2:$P$52,,MATCH( A92&amp;"_rank",$A$1:$P$1,0)),$A$2:$A$52)</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="E92" s="5" cm="1">
+        <f t="array" ref="E92">_xlfn.XLOOKUP($D$89,INDEX($A$2:$P$52,,MATCH( A92&amp;"_rank",$A$1:$P$1,0)),INDEX($A$2:$P$52,,MATCH(A92&amp;"_diff_pct",$A$1:$P$1,0)))</f>
+        <v>-0.17103239309050916</v>
+      </c>
+      <c r="F92" t="str" cm="1">
+        <f t="array" ref="F92">_xlfn.XLOOKUP($F$89,INDEX($A$2:$P$52,,MATCH( A92&amp;"_rank",$A$1:$P$1,0)),$A$2:$A$52)</f>
+        <v>Office of Family Safety</v>
+      </c>
+      <c r="G92" s="5" cm="1">
+        <f t="array" ref="G92">_xlfn.XLOOKUP($F$89,INDEX($A$2:$P$52,,MATCH( A92&amp;"_rank",$A$1:$P$1,0)),INDEX($A$2:$P$52,,MATCH(A92&amp;"_diff_pct",$A$1:$P$1,0)))</f>
+        <v>-0.13918241656366656</v>
+      </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>75</v>
       </c>
-      <c r="C93" s="5"/>
-      <c r="E93" s="5"/>
-      <c r="G93" s="5"/>
+      <c r="B93" t="str" cm="1">
+        <f t="array" ref="B93">_xlfn.XLOOKUP($B$89,INDEX($A$2:$P$52,,MATCH( A93&amp;"_rank",$A$1:$P$1,0)),$A$2:$A$52)</f>
+        <v>Community Oversight Board</v>
+      </c>
+      <c r="C93" s="5" cm="1">
+        <f t="array" ref="C93">_xlfn.XLOOKUP($B$89,INDEX($A$2:$P$52,,MATCH( A93&amp;"_rank",$A$1:$P$1,0)),INDEX($A$2:$P$52,,MATCH(A93&amp;"_diff_pct",$A$1:$P$1,0)))</f>
+        <v>-0.82994157333333329</v>
+      </c>
+      <c r="D93" t="str" cm="1">
+        <f t="array" ref="D93">_xlfn.XLOOKUP($D$89,INDEX($A$2:$P$52,,MATCH( A93&amp;"_rank",$A$1:$P$1,0)),$A$2:$A$52)</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="E93" s="5" cm="1">
+        <f t="array" ref="E93">_xlfn.XLOOKUP($D$89,INDEX($A$2:$P$52,,MATCH( A93&amp;"_rank",$A$1:$P$1,0)),INDEX($A$2:$P$52,,MATCH(A93&amp;"_diff_pct",$A$1:$P$1,0)))</f>
+        <v>-0.15295680364719175</v>
+      </c>
+      <c r="F93" t="str" cm="1">
+        <f t="array" ref="F93">_xlfn.XLOOKUP($F$89,INDEX($A$2:$P$52,,MATCH( A93&amp;"_rank",$A$1:$P$1,0)),$A$2:$A$52)</f>
+        <v>Election Commission</v>
+      </c>
+      <c r="G93" s="5" cm="1">
+        <f t="array" ref="G93">_xlfn.XLOOKUP($F$89,INDEX($A$2:$P$52,,MATCH( A93&amp;"_rank",$A$1:$P$1,0)),INDEX($A$2:$P$52,,MATCH(A93&amp;"_diff_pct",$A$1:$P$1,0)))</f>
+        <v>-0.12882667147667154</v>
+      </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="7" t="s">
@@ -5814,27 +5898,90 @@
       <c r="A98" t="s">
         <v>73</v>
       </c>
-      <c r="C98" s="4"/>
-      <c r="E98" s="4"/>
-      <c r="G98" s="4"/>
+      <c r="B98" t="str">
+        <f>INDEX($A$2:$A$52,MATCH($B$96,INDEX($A$2:$P$52,,MATCH(A98&amp;"_rank",$A$1:$P$1,0)),0))</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="C98" s="4">
+        <f>INDEX($A$2:$P$52,MATCH($B$96,INDEX($A$2:$P$52,,MATCH(A98&amp;"_rank",$A$1:$P$1,0)),0),MATCH(A98&amp;"_diff_pct",$A$1:$P$1,0))</f>
+        <v>-0.15235918433091292</v>
+      </c>
+      <c r="D98" t="str">
+        <f>INDEX($A$2:$A$52,MATCH($D$96,INDEX($A$2:$P$52,,MATCH(A98&amp;"_rank",$A$1:$P$1,0)),0))</f>
+        <v>Circuit Court Clerk</v>
+      </c>
+      <c r="E98" s="4">
+        <f>INDEX($A$2:$P$52,MATCH($D$96,INDEX($A$2:$P$52,,MATCH(A98&amp;"_rank",$A$1:$P$1,0)),0),MATCH(A98&amp;"_diff_pct",$A$1:$P$1,0))</f>
+        <v>-0.11502817362571344</v>
+      </c>
+      <c r="F98" t="str">
+        <f>INDEX($A$2:$A$52,MATCH($F$96,INDEX($A$2:$P$52,,MATCH(A98&amp;"_rank",$A$1:$P$1,0)),0))</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="G98" s="4">
+        <f>INDEX($A$2:$P$52,MATCH($F$96,INDEX($A$2:$P$52,,MATCH(A98&amp;"_rank",$A$1:$P$1,0)),0),MATCH(A98&amp;"_diff_pct",$A$1:$P$1,0))</f>
+        <v>-9.5782760864849215E-2</v>
+      </c>
       <c r="I98" s="4"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>74</v>
       </c>
-      <c r="C99" s="4"/>
-      <c r="E99" s="4"/>
-      <c r="G99" s="4"/>
+      <c r="B99" t="str">
+        <f t="shared" ref="B99:B100" si="14">INDEX($A$2:$A$52,MATCH($B$96,INDEX($A$2:$P$52,,MATCH(A99&amp;"_rank",$A$1:$P$1,0)),0))</f>
+        <v>Metropolitan Clerk</v>
+      </c>
+      <c r="C99" s="4">
+        <f t="shared" ref="C99:C100" si="15">INDEX($A$2:$P$52,MATCH($B$96,INDEX($A$2:$P$52,,MATCH(A99&amp;"_rank",$A$1:$P$1,0)),0),MATCH(A99&amp;"_diff_pct",$A$1:$P$1,0))</f>
+        <v>-0.17551246244575608</v>
+      </c>
+      <c r="D99" t="str">
+        <f t="shared" ref="D99:D100" si="16">INDEX($A$2:$A$52,MATCH($D$96,INDEX($A$2:$P$52,,MATCH(A99&amp;"_rank",$A$1:$P$1,0)),0))</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="E99" s="4">
+        <f t="shared" ref="E99:E100" si="17">INDEX($A$2:$P$52,MATCH($D$96,INDEX($A$2:$P$52,,MATCH(A99&amp;"_rank",$A$1:$P$1,0)),0),MATCH(A99&amp;"_diff_pct",$A$1:$P$1,0))</f>
+        <v>-0.17103239309050916</v>
+      </c>
+      <c r="F99" t="str">
+        <f t="shared" ref="F99:F100" si="18">INDEX($A$2:$A$52,MATCH($F$96,INDEX($A$2:$P$52,,MATCH(A99&amp;"_rank",$A$1:$P$1,0)),0))</f>
+        <v>Office of Family Safety</v>
+      </c>
+      <c r="G99" s="4">
+        <f t="shared" ref="G99:G100" si="19">INDEX($A$2:$P$52,MATCH($F$96,INDEX($A$2:$P$52,,MATCH(A99&amp;"_rank",$A$1:$P$1,0)),0),MATCH(A99&amp;"_diff_pct",$A$1:$P$1,0))</f>
+        <v>-0.13918241656366656</v>
+      </c>
       <c r="I99" s="4"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>75</v>
       </c>
-      <c r="C100" s="4"/>
-      <c r="E100" s="4"/>
-      <c r="G100" s="4"/>
+      <c r="B100" t="str">
+        <f t="shared" si="14"/>
+        <v>Community Oversight Board</v>
+      </c>
+      <c r="C100" s="4">
+        <f t="shared" si="15"/>
+        <v>-0.82994157333333329</v>
+      </c>
+      <c r="D100" t="str">
+        <f t="shared" si="16"/>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="E100" s="4">
+        <f t="shared" si="17"/>
+        <v>-0.15295680364719175</v>
+      </c>
+      <c r="F100" t="str">
+        <f t="shared" si="18"/>
+        <v>Election Commission</v>
+      </c>
+      <c r="G100" s="4">
+        <f t="shared" si="19"/>
+        <v>-0.12882667147667154</v>
+      </c>
       <c r="I100" s="4"/>
     </row>
   </sheetData>

</xml_diff>